<commit_message>
Implement writeemail, bugs identified in README.md
</commit_message>
<xml_diff>
--- a/data/emailCollection.xlsx
+++ b/data/emailCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chell\Documents\GitHub\EmailWebApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2779F707-990C-41BE-91EB-D2481C24598B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1FE2F5-B452-4CE6-9084-45BB38E1FD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -85,6 +85,9 @@
     <t>The id of this email should be 3. Email saved as draft again! Now it has been sent.</t>
   </si>
   <si>
+    <t>{No Subject}</t>
+  </si>
+  <si>
     <t>This is my first draft. The ID should be 4. Draft Updated and sent!</t>
   </si>
   <si>
@@ -118,7 +121,16 @@
     <t>AGAIN I sent yet ANOTHER email via postman</t>
   </si>
   <si>
-    <t>{No Subject}</t>
+    <t>Postman4</t>
+  </si>
+  <si>
+    <t>Postman5</t>
+  </si>
+  <si>
+    <t>updated AGAIN I sent yet ANOTHER email via postman</t>
+  </si>
+  <si>
+    <t>Postman6</t>
   </si>
 </sst>
 </file>
@@ -485,16 +497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-    <col min="4" max="4" width="21.90625" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -647,13 +658,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2">
         <v>44962.571527777778</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
@@ -676,13 +687,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2">
         <v>44962.575694444437</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
@@ -705,13 +716,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2">
         <v>44974.992361111108</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
@@ -734,13 +745,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2">
         <v>44975.014120370368</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
@@ -749,10 +760,10 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -763,13 +774,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2">
         <v>44975.014120370368</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -784,6 +795,93 @@
         <v>14</v>
       </c>
       <c r="I10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2">
+        <v>25569.019386574073</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2">
+        <v>25569.019386574073</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>25569.019389594909</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove requirement for ID from client
</commit_message>
<xml_diff>
--- a/data/emailCollection.xlsx
+++ b/data/emailCollection.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -900,11 +900,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Postman5</t>
+          <t>Postman5PT2</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>25569.01938657407</v>
+        <v>44958.59311342592</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1014,6 +1014,47 @@
         </is>
       </c>
       <c r="I14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Saving new email 2</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Hope this works AGAIN!</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>{No Recipient Email}</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>{No Recipient Name}</t>
+        </is>
+      </c>
+      <c r="I15" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement save and send emails JS
Fully implement write new emails, edit draft, save as draft, and send draft or new mail on js side
</commit_message>
<xml_diff>
--- a/data/emailCollection.xlsx
+++ b/data/emailCollection.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1058,6 +1058,88 @@
         <v>1</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>First email via app</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>44992.729375</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Wish me luck!</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>marleevaughn@outlook.com</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Marlee Vaughn</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>First draft</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>44992.73216435185</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>My first draft via app has been edited ONCE! and has id of 15 and has now been sent</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>marleevaughn@outlook.com</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Marlee Vaughn</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>kalevaughn@gmail.com</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Kale Vaughn</t>
+        </is>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor sys api calls
Condense sys api calls to use usable functions to make code drier.
Introduce .env file to use for later
</commit_message>
<xml_diff>
--- a/data/emailCollection.xlsx
+++ b/data/emailCollection.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,7 +777,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Postman2UPDATE2</t>
+          <t>Postman2UPDATE2UPDATE2</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -900,7 +900,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Postman5PT2</t>
+          <t>Postman5PT3</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1138,6 +1138,170 @@
       </c>
       <c r="I17" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Postman10</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>AGAIN I sent yet ANOTHER email via postman</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>marleevaughn@outlook.com</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Marlee Vaughn</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Postman10</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>AGAIN I sent yet ANOTHER email via postman</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>marleevaughn@outlook.com</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Marlee Vaughn</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Postman11</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>AGAIN I sent yet ANOTHER email via postman</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>marleevaughn@outlook.com</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Marlee Vaughn</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Saving new email 3</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Hope this works AGAIN!</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>{No Recipient Email}</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>{No Recipient Name}</t>
+        </is>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make python files dry
Make all python files dry
</commit_message>
<xml_diff>
--- a/data/emailCollection.xlsx
+++ b/data/emailCollection.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,7 +539,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Hey sis!</t>
+          <t>Hey sis! I've updated this email on 22/3/23</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -900,7 +900,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Postman5PT3</t>
+          <t>Postman5PT7</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1383,6 +1383,375 @@
         </is>
       </c>
       <c r="I23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Postman69</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>44958.59311342592</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>AGAIN I sent yet ANOTHER email via postman</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>marleevaughn@outlook.com</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Marlee Vaughn</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Postman9</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>44958.59311342592</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>AGAIN I sent yet ANOTHER email via postman</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>marleevaughn@outlook.com</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Marlee Vaughn</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Saving new email 093</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Hope this works AGAIN!</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>{No Recipient Email}</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>{No Recipient Name}</t>
+        </is>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Saving new email 123</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Hope this works AGAIN!</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>{No Recipient Email}</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>{No Recipient Name}</t>
+        </is>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Saving new email 123</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Hope this works AGAIN!</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>{No Recipient Email}</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>{No Recipient Name}</t>
+        </is>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Saving new email 1234</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Hope this works AGAIN!</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>{No Recipient Email}</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>{No Recipient Name}</t>
+        </is>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Saving new email 4321</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Hope this works AGAIN!</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>{No Recipient Email}</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>{No Recipient Name}</t>
+        </is>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Saving new email 135</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Hope this works AGAIN!</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>{No Recipient Email}</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>{No Recipient Name}</t>
+        </is>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Saving new email 1357</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>44958.59305555555</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Hope this works AGAIN!</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>duanevaughn@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Duane Vaughn</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>{No Recipient Email}</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>{No Recipient Name}</t>
+        </is>
+      </c>
+      <c r="I32" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
make email fields lowercase on submit
Make email fields lowercase on submit from js perspective. Fix bug on ewa_expapi_func.py
</commit_message>
<xml_diff>
--- a/data/emailCollection.xlsx
+++ b/data/emailCollection.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1755,6 +1755,170 @@
         <v>1</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Hi Luke</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>45009.48006944444</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>This is my first email as the developer.</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>chelly-xox@hotmail.co.uk</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Micah Chuku</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>lukevaughn@aol.com</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Luke Vaughn</t>
+        </is>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Hi again, Luke</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>45009.48297453704</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>'Sup bro?</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>chelly-xox@hotmail.co.uk</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Micah Chuku</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>lukevaughn@aol.com</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Luke Vaughn</t>
+        </is>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Hello Luke</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>45009.48892361111</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>I am writing this email with your email address capitalised. Hopefully the web app should turn this to lowercase before submitting to the API. Have a good day!</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>n.schneider@gmail.com</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Natalia Schneider</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>lukevaughn@aol.com</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Luke Vaughn</t>
+        </is>
+      </c>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Hi again again</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>45009.49577546296</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Testing out after removing patter on email field</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>chelly-xox@hotmail.co.uk</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Micah Chuku</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>lukevaughn@aol.com</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Luke Vaughn</t>
+        </is>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>